<commit_message>
escape shellwords on image export
</commit_message>
<xml_diff>
--- a/public/downloads/1/giveaway.xlsx
+++ b/public/downloads/1/giveaway.xlsx
@@ -9,7 +9,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="60">
   <si>
     <t>Brand</t>
   </si>
@@ -38,10 +38,157 @@
     <t>NLL00 – Alpine Snow</t>
   </si>
   <si>
+    <t>Launch</t>
+  </si>
+  <si>
     <t>1989</t>
   </si>
   <si>
     <t>light</t>
+  </si>
+  <si>
+    <t>Bobo</t>
+  </si>
+  <si>
+    <t>green sand</t>
+  </si>
+  <si>
+    <t>green</t>
+  </si>
+  <si>
+    <t>CHANEL</t>
+  </si>
+  <si>
+    <t>543 – Frision</t>
+  </si>
+  <si>
+    <t>yellow</t>
+  </si>
+  <si>
+    <t>orly</t>
+  </si>
+  <si>
+    <t>gfgfg</t>
+  </si>
+  <si>
+    <t>new orleans</t>
+  </si>
+  <si>
+    <t>2014</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>np653</t>
+  </si>
+  <si>
+    <t>turquoise</t>
+  </si>
+  <si>
+    <t>LaPierre</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>ivory</t>
+  </si>
+  <si>
+    <t>evixi</t>
+  </si>
+  <si>
+    <t>Blooming Violet</t>
+  </si>
+  <si>
+    <t>Firecracker</t>
+  </si>
+  <si>
+    <t>Earth Spice</t>
+  </si>
+  <si>
+    <t>Crimson Tide</t>
+  </si>
+  <si>
+    <t>Birthday Suit</t>
+  </si>
+  <si>
+    <t>Clove</t>
+  </si>
+  <si>
+    <t>DS Temptation</t>
+  </si>
+  <si>
+    <t>Guatemala Guava</t>
+  </si>
+  <si>
+    <t>Have a Tempera Tan-Trum</t>
+  </si>
+  <si>
+    <t>Hot Chocolate</t>
+  </si>
+  <si>
+    <t>Dawn to Dusk</t>
+  </si>
+  <si>
+    <t>Yellin’ For Watermelon</t>
+  </si>
+  <si>
+    <t>Emerald Envy</t>
+  </si>
+  <si>
+    <t>Coral Treasure</t>
+  </si>
+  <si>
+    <t>Pacific Green</t>
+  </si>
+  <si>
+    <t>535 May</t>
+  </si>
+  <si>
+    <t>587 Rouge Carat</t>
+  </si>
+  <si>
+    <t>Fantastic 481</t>
+  </si>
+  <si>
+    <t>Cafe Latte</t>
+  </si>
+  <si>
+    <t>Licorice</t>
+  </si>
+  <si>
+    <t>Lapis Lazuli</t>
+  </si>
+  <si>
+    <t>Holographic</t>
+  </si>
+  <si>
+    <t>18 Rouge Noir</t>
+  </si>
+  <si>
+    <t>Orange Sunshine</t>
+  </si>
+  <si>
+    <t>473 Corormandel</t>
+  </si>
+  <si>
+    <t>Perfectly Pink</t>
+  </si>
+  <si>
+    <t>Lovely Lilac</t>
+  </si>
+  <si>
+    <t>Pink Candy</t>
+  </si>
+  <si>
+    <t>Red Dream</t>
+  </si>
+  <si>
+    <t>Taboo</t>
+  </si>
+  <si>
+    <t>April</t>
   </si>
 </sst>
 </file>
@@ -52,7 +199,7 @@
     <numFmt numFmtId="100" formatCode="yyyy/mm/dd"/>
     <numFmt numFmtId="101" formatCode="yyyy/mm/dd hh:mm:ss"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="8">
     <font>
       <name val="Arial"/>
       <sz val="11"/>
@@ -71,8 +218,38 @@
       <family val="1"/>
       <color rgb="FF000000"/>
     </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="11"/>
+      <family val="1"/>
+      <color rgb="FFFFFFFF"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="11"/>
+      <family val="1"/>
+      <color rgb="FFFFFFFF"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="11"/>
+      <family val="1"/>
+      <color rgb="FFFFFFFF"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="11"/>
+      <family val="1"/>
+      <color rgb="FFFFFFFF"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="11"/>
+      <family val="1"/>
+      <color rgb="FF000000"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -87,6 +264,31 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF5B5B5B"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF1B850F"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFD500"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD60000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0D5E5C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFEB3"/>
       </patternFill>
     </fill>
   </fills>
@@ -110,7 +312,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" numFmtId="0" fontId="0" fillId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf borderId="0" numFmtId="0" fontId="0" fillId="0" xfId="0"/>
     <xf borderId="1" numFmtId="0" fontId="0" fillId="0" xfId="0"/>
     <xf borderId="0" numFmtId="14" fontId="0" fillId="0" xfId="0" applyNumberFormat="1"/>
@@ -118,6 +320,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="0" numFmtId="0" fontId="2" fillId="3" applyNumberFormat="false" applyFill="true" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="0" numFmtId="0" fontId="3" fillId="4" applyNumberFormat="false" applyFill="true" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="0" numFmtId="0" fontId="4" fillId="5" applyNumberFormat="false" applyFill="true" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="0" numFmtId="0" fontId="5" fillId="6" applyNumberFormat="false" applyFill="true" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="0" numFmtId="0" fontId="6" fillId="7" applyNumberFormat="false" applyFill="true" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="0" numFmtId="0" fontId="7" fillId="8" applyNumberFormat="false" applyFill="true" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -134,7 +351,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0">
       <pane topLeftCell="A2" state="frozen" ySplit="1" xSplit="0"/>
@@ -143,7 +360,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="12.198876404494383"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="19.58988764044944"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="20.68988764044944"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="16.398876404494384"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="10.098876404494384"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="14.298876404494383"/>
@@ -181,18 +398,404 @@
       <c r="B2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="0"/>
+      <c r="C2" s="0" t="s">
+        <v>9</v>
+      </c>
       <c r="D2" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>10</v>
-      </c>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="0"/>
+      <c r="D3" s="0"/>
+      <c r="E3" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="0"/>
+      <c r="D4" s="0"/>
+      <c r="E4" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="0"/>
+      <c r="D6" s="0"/>
+      <c r="E6" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="0"/>
+      <c r="D7" s="0"/>
+      <c r="E7" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="0"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="0"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="0"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="0"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="0"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="0"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="0"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="0"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="0"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="0"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="0"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="0"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="0"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="0"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="0"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="0"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="0"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="0"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" s="0"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" s="0"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" s="0"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29" s="0"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="C30" s="0"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31" s="0"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C32" s="0"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="C33" s="0"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C34" s="0"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="C35" s="0"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="C36" s="0"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="C37" s="0"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="C38" s="0"/>
     </row>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="true"/>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="B5" r:id="rId4"/>
+    <hyperlink ref="B6" r:id="rId5"/>
+    <hyperlink ref="B7" r:id="rId6"/>
+    <hyperlink ref="B8" r:id="rId7"/>
+    <hyperlink ref="B9" r:id="rId8"/>
+    <hyperlink ref="B10" r:id="rId9"/>
+    <hyperlink ref="B11" r:id="rId10"/>
+    <hyperlink ref="B12" r:id="rId11"/>
+    <hyperlink ref="B13" r:id="rId12"/>
+    <hyperlink ref="B14" r:id="rId13"/>
+    <hyperlink ref="B15" r:id="rId14"/>
+    <hyperlink ref="B16" r:id="rId15"/>
+    <hyperlink ref="B17" r:id="rId16"/>
+    <hyperlink ref="B18" r:id="rId17"/>
+    <hyperlink ref="B19" r:id="rId18"/>
+    <hyperlink ref="B20" r:id="rId19"/>
+    <hyperlink ref="B21" r:id="rId20"/>
+    <hyperlink ref="B22" r:id="rId21"/>
+    <hyperlink ref="B23" r:id="rId22"/>
+    <hyperlink ref="B24" r:id="rId23"/>
+    <hyperlink ref="B25" r:id="rId24"/>
+    <hyperlink ref="B26" r:id="rId25"/>
+    <hyperlink ref="B27" r:id="rId26"/>
+    <hyperlink ref="B28" r:id="rId27"/>
+    <hyperlink ref="B29" r:id="rId28"/>
+    <hyperlink ref="B30" r:id="rId29"/>
+    <hyperlink ref="B31" r:id="rId30"/>
+    <hyperlink ref="B32" r:id="rId31"/>
+    <hyperlink ref="B33" r:id="rId32"/>
+    <hyperlink ref="B34" r:id="rId33"/>
+    <hyperlink ref="B35" r:id="rId34"/>
+    <hyperlink ref="B36" r:id="rId35"/>
+    <hyperlink ref="B37" r:id="rId36"/>
+    <hyperlink ref="B38" r:id="rId37"/>
   </hyperlinks>
   <printOptions verticalCentered="false" horizontalCentered="false" headings="false" gridLines="false"/>
   <pageMargins right="0.75" left="0.75" bottom="1.0" top="1.0" footer="0.5" header="0.5"/>

</xml_diff>